<commit_message>
fix mistake from unexposed prevalences in brm agg models
</commit_message>
<xml_diff>
--- a/out/dataframes/brm_results_agg.xlsx
+++ b/out/dataframes/brm_results_agg.xlsx
@@ -417,12 +417,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NaN%</t>
+          <t>14.9%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>14.9%</t>
+          <t>38.9%</t>
         </is>
       </c>
       <c r="G2">
@@ -452,12 +452,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>NaN%</t>
+          <t>18.3%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>18.3%</t>
+          <t>41.5%</t>
         </is>
       </c>
       <c r="G3">
@@ -487,12 +487,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NaN%</t>
+          <t>16.8%</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>16.8%</t>
+          <t>38.7%</t>
         </is>
       </c>
       <c r="G4">
@@ -522,12 +522,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>NaN%</t>
+          <t>19.4%</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>19.4%</t>
+          <t>40.7%</t>
         </is>
       </c>
       <c r="G5">
@@ -557,12 +557,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>NaN%</t>
+          <t>21.2%</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>21.2%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="G6">
@@ -592,12 +592,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>NaN%</t>
+          <t>26.0%</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>26.0%</t>
+          <t>54.3%</t>
         </is>
       </c>
       <c r="G7">
@@ -627,12 +627,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>NaN%</t>
+          <t>23.8%</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>23.8%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="G8">
@@ -662,12 +662,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>NaN%</t>
+          <t>27.4%</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>27.4%</t>
+          <t>53.2%</t>
         </is>
       </c>
       <c r="G9">

</xml_diff>